<commit_message>
Bunch of changes. Added runeball 2020
</commit_message>
<xml_diff>
--- a/SupersNew/characters/Jack.xlsx
+++ b/SupersNew/characters/Jack.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rb\SupersNew\characters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magou\Desktop\Runebearer\SupersNew\characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EDAF0D-974F-492A-8028-FF98600F30C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="12690" yWindow="0" windowWidth="25500" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Character Sheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="PowersTest" sheetId="5" r:id="rId5"/>
     <sheet name="Character Sheet Test" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,8 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -913,11 +916,42 @@
     <t>Fire Blast</t>
   </si>
   <si>
+    <t>Careless</t>
+  </si>
+  <si>
+    <t>Fire Flight</t>
+  </si>
+  <si>
+    <t>Fire Immunity</t>
+  </si>
+  <si>
+    <t>Flamethrower</t>
+  </si>
+  <si>
+    <t>Ats</t>
+  </si>
+  <si>
+    <t>3 cone</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>Stimulant</t>
+  </si>
+  <si>
+    <t>Iron Liver</t>
+  </si>
+  <si>
+    <t>Trait</t>
+  </si>
+  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -927,12 +961,13 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
         <family val="2"/>
       </rPr>
-      <t>2d10 + Skill energy damage</t>
+      <t>You take no penalty when firing into melee, but your chance to hit allies in 4/12</t>
     </r>
   </si>
   <si>
@@ -941,6 +976,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -950,16 +986,14 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
         <family val="2"/>
       </rPr>
-      <t>Ignite(3)</t>
+      <t>2d10 + Skill energy damage</t>
     </r>
-  </si>
-  <si>
-    <t>Careless</t>
   </si>
   <si>
     <r>
@@ -967,6 +1001,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -976,16 +1011,14 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
         <family val="2"/>
       </rPr>
-      <t>You take no penalty when firing into melee, but your chance to hit allies in 4/12</t>
+      <t>Ignite(3)</t>
     </r>
-  </si>
-  <si>
-    <t>Fire Flight</t>
   </si>
   <si>
     <r>
@@ -993,6 +1026,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1002,6 +1036,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1011,14 +1046,12 @@
     </r>
   </si>
   <si>
-    <t>Fire Immunity</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1028,6 +1061,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1042,6 +1076,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1051,6 +1086,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1060,20 +1096,12 @@
     </r>
   </si>
   <si>
-    <t>Flamethrower</t>
-  </si>
-  <si>
-    <t>Ats</t>
-  </si>
-  <si>
-    <t>3 cone</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1083,6 +1111,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1097,6 +1126,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1106,6 +1136,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1115,14 +1146,12 @@
     </r>
   </si>
   <si>
-    <t>Booster</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1132,6 +1161,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1141,14 +1171,12 @@
     </r>
   </si>
   <si>
-    <t>Stimulant</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1158,6 +1186,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1172,6 +1201,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1181,6 +1211,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1195,6 +1226,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1204,6 +1236,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1218,6 +1251,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1227,6 +1261,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1241,6 +1276,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1250,6 +1286,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1264,6 +1301,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1273,6 +1311,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1287,6 +1326,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1296,6 +1336,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1305,17 +1346,12 @@
     </r>
   </si>
   <si>
-    <t>Iron Liver</t>
-  </si>
-  <si>
-    <t>Trait</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1325,6 +1361,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1339,6 +1376,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -1348,6 +1386,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Abadi"/>
@@ -1360,8 +1399,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1422,10 +1461,26 @@
       <charset val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Abadi"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1657,45 +1712,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1717,6 +1733,45 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2192,11 +2247,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,13 +2273,13 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
@@ -2232,11 +2290,11 @@
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="10" t="s">
         <v>33</v>
       </c>
@@ -2459,8 +2517,8 @@
       <c r="D14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="9" t="s">
         <v>77</v>
       </c>
@@ -2477,7 +2535,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="37"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -2492,7 +2550,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="37"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2540,403 +2598,391 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="33">
+        <v>10</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+      <c r="I19" s="35" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="36">
+        <v>20</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="36">
+        <v>0</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="36">
+        <v>6</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="41" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="33">
+        <v>20</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="H22" s="33">
+        <v>1</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B23" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C23" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D23" s="36">
         <v>10</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E23" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F23" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="G23" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H23" s="36">
         <v>0</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="I23" s="38" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="41" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>280</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" s="31" t="s">
+      <c r="B25" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D25" s="36">
         <v>20</v>
       </c>
-      <c r="E20" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="F20" s="31">
+      <c r="E25" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="H25" s="36">
+        <v>8</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="41" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="33">
+        <v>20</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F28" s="33">
         <v>0</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G28" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H28" s="33">
         <v>6</v>
       </c>
-      <c r="I20" s="24" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="25" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="D22" s="27">
+      <c r="I28" s="35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="D29" s="36">
         <v>20</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E29" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F29" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G29" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="H29" s="36">
+        <v>7</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="44" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="44" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="44" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="44" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="42"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="41" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="D36" s="36">
+        <v>10</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="G36" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="H22" s="27">
-        <v>1</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>287</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="D23" s="31">
-        <v>10</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="H23" s="31">
+      <c r="H36" s="36">
         <v>0</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>291</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="D25" s="31">
-        <v>20</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="G25" s="33" t="s">
-        <v>292</v>
-      </c>
-      <c r="H25" s="31">
-        <v>8</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="30" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="25" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="D28" s="27">
-        <v>20</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="F28" s="27">
-        <v>0</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="H28" s="27">
-        <v>6</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="D29" s="31">
-        <v>20</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F29" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="H29" s="31">
-        <v>7</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="30" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="30" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="30" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="30" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="30" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="25" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>305</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>306</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="31">
-        <v>10</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="G36" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="H36" s="31">
-        <v>0</v>
-      </c>
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="38" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="25" t="s">
+    <row r="37" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="41" t="s">
         <v>308</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="G25:G27"/>
     <mergeCell ref="H25:H27"/>
@@ -2953,27 +2999,39 @@
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Fighting Profiles'!$A$2:$A$48</xm:f>
           </x14:formula1>
           <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Power Sets'!$A$2:$A$48</xm:f>
           </x14:formula1>
@@ -2986,7 +3044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3239,7 +3297,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A48">
     <sortCondition ref="A48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3247,7 +3305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4701,7 +4759,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4709,7 +4767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -4730,11 +4788,11 @@
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
@@ -5159,7 +5217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -5206,28 +5264,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="28">
         <v>20</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="28">
         <v>1</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="28">
         <v>4</v>
       </c>
       <c r="I4" s="20" t="s">
@@ -5235,27 +5293,27 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="20" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="19" t="s">
         <v>256</v>
       </c>
@@ -5290,28 +5348,28 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="28">
         <v>20</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="28">
         <v>1</v>
       </c>
       <c r="I8" s="20" t="s">
@@ -5319,41 +5377,41 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="20" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="28">
         <v>10</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="28">
         <v>0</v>
       </c>
       <c r="I10" s="20" t="s">
@@ -5361,14 +5419,14 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="189" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="20" t="s">
         <v>263</v>
       </c>
@@ -5403,28 +5461,28 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="28">
         <v>20</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="28">
         <v>0</v>
       </c>
       <c r="I13" s="20" t="s">
@@ -5432,14 +5490,14 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="20" t="s">
         <v>266</v>
       </c>
@@ -5474,28 +5532,28 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="28">
         <v>20</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="H16" s="41">
+      <c r="H16" s="28">
         <v>2</v>
       </c>
       <c r="I16" s="20" t="s">
@@ -5503,27 +5561,27 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="20" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="20" t="s">
         <v>270</v>
       </c>
@@ -5616,28 +5674,28 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="28">
         <v>20</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="H22" s="41">
+      <c r="H22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="23" t="s">
@@ -5645,27 +5703,27 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="20" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="20" t="s">
         <v>276</v>
       </c>
@@ -5730,6 +5788,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="A10:A11"/>
@@ -5746,45 +5836,13 @@
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5807,11 +5865,11 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
@@ -5822,11 +5880,11 @@
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="10" t="s">
         <v>80</v>
       </c>
@@ -6059,8 +6117,8 @@
       <c r="D15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="9" t="s">
         <v>77</v>
       </c>
@@ -6077,7 +6135,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="37"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -6092,7 +6150,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="37"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -6102,17 +6160,17 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="37"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="43"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -6133,26 +6191,26 @@
       <c r="A21" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="44" t="str">
+      <c r="B21" s="31" t="str">
         <f>VLOOKUP(B19,'Day Jobs'!A3:F15,3,FALSE)</f>
         <v>Improvise (CW), Perform (CW), Lie (CW), Crafty (RS)</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="42" t="str">
+      <c r="B22" s="29" t="str">
         <f>VLOOKUP(B19,'Day Jobs'!A3:F15,4,FALSE)</f>
         <v>Big Personality</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -6163,21 +6221,21 @@
       <c r="A23" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B23" s="42" t="str">
+      <c r="B23" s="29" t="str">
         <f>VLOOKUP(B19,'Day Jobs'!A3:F15,5,FALSE)</f>
         <v>Quick Change</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B24" s="42" t="str">
+      <c r="B24" s="29" t="str">
         <f>VLOOKUP(B19,'Day Jobs'!A3:F15,6,FALSE)</f>
         <v>Star Material</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -6250,19 +6308,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>'Power Sets'!$A$2:$A$48</xm:f>
           </x14:formula1>
           <xm:sqref>B3:C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
           <x14:formula1>
             <xm:f>'Day Jobs'!$A$4:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>B19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>
             <xm:f>'Fighting Profiles'!$A$2:$A$48</xm:f>
           </x14:formula1>

</xml_diff>